<commit_message>
anexo de requerimientos, al crear el calendario, ahora se preserva el logo, igualmente se muestra la sede y hora del examen
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\flask-calendar\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greed\Documents\flask-calendar\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">CALENDARIO DE EXÁMENES </t>
   </si>
@@ -54,34 +54,13 @@
     <t>Ordinario</t>
   </si>
   <si>
-    <t>Recuperativo</t>
-  </si>
-  <si>
-    <t>Especial</t>
-  </si>
-  <si>
     <t>Entrega de Calificaciones</t>
   </si>
   <si>
-    <t>Negociación Empresarial</t>
-  </si>
-  <si>
-    <t>Auditoría de Sistemas de TI</t>
-  </si>
-  <si>
-    <t>Estadística Aplicada</t>
-  </si>
-  <si>
-    <t>Seguridad de la Información</t>
-  </si>
-  <si>
-    <t>Integradora II</t>
-  </si>
-  <si>
-    <t>Tópicos Selectos de TI</t>
-  </si>
-  <si>
-    <t>Ingles VI</t>
+    <t>Extraordinario 1</t>
+  </si>
+  <si>
+    <t>Extraordinario 2</t>
   </si>
 </sst>
 </file>
@@ -236,12 +215,6 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -299,6 +272,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,8 +414,8 @@
     <tableColumn id="3" name="Segundo Periodo"/>
     <tableColumn id="4" name="Tercer Periodo"/>
     <tableColumn id="5" name="Ordinario"/>
-    <tableColumn id="6" name="Recuperativo"/>
-    <tableColumn id="7" name="Especial"/>
+    <tableColumn id="6" name="Extraordinario 1"/>
+    <tableColumn id="7" name="Extraordinario 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,243 +690,237 @@
   <dimension ref="A1:AMK44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="G15" sqref="A6:G15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="38.7109375" style="3" customWidth="1"/>
-    <col min="8" max="1025" width="10.7109375" style="3"/>
+    <col min="1" max="1" width="45.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="32.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="1" customWidth="1"/>
+    <col min="8" max="1025" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="4"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="4"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>43377</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>43410</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>43440</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>43447</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>43474</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>43474</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="17"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="35" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="23"/>
+      <c r="A35" s="21"/>
     </row>
     <row r="36" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="23"/>
+      <c r="A36" s="21"/>
     </row>
     <row r="37" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A37" s="23"/>
+      <c r="A37" s="21"/>
     </row>
     <row r="38" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="23"/>
+      <c r="A38" s="21"/>
     </row>
     <row r="39" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21"/>
     </row>
     <row r="40" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="23"/>
+      <c r="A40" s="21"/>
     </row>
     <row r="41" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A41" s="23"/>
+      <c r="A41" s="21"/>
     </row>
     <row r="42" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="23"/>
+      <c r="A42" s="21"/>
     </row>
     <row r="43" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A43" s="23"/>
+      <c r="A43" s="21"/>
     </row>
     <row r="44" spans="1:1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
+      <c r="A44" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>